<commit_message>
Terminal web extraction file modified
</commit_message>
<xml_diff>
--- a/Ops Assist/Terminal_web_Extraction/Operator wise vessel details.xlsx
+++ b/Ops Assist/Terminal_web_Extraction/Operator wise vessel details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssc.achauhan\Desktop\Projects\Ops Assist\Terminal_web_Extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93629A3-689F-4B5A-A09F-F6E244608BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA35760-9DAD-4028-B069-3C6CAE1C551F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{89783E6D-8C4E-4785-A8DE-D4DADDE5902E}"/>
   </bookViews>
@@ -3236,12 +3236,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3250,6 +3244,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9612,10 +9612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6CD1FA5-7C40-4123-BBCD-AB20E1A16CDA}">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J551"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -9668,7 +9668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -9691,7 +9691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -9714,7 +9714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>16</v>
       </c>
@@ -9737,7 +9737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>17</v>
       </c>
@@ -9760,7 +9760,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>18</v>
       </c>
@@ -9783,7 +9783,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>19</v>
       </c>
@@ -9806,7 +9806,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>20</v>
       </c>
@@ -9829,7 +9829,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>21</v>
       </c>
@@ -9852,7 +9852,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>22</v>
       </c>
@@ -9875,7 +9875,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>23</v>
       </c>
@@ -9898,7 +9898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>24</v>
       </c>
@@ -9921,7 +9921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>25</v>
       </c>
@@ -9944,7 +9944,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>26</v>
       </c>
@@ -9967,7 +9967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>27</v>
       </c>
@@ -9990,7 +9990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>28</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>29</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>30</v>
       </c>
@@ -10059,7 +10059,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>31</v>
       </c>
@@ -10082,7 +10082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>32</v>
       </c>
@@ -10105,7 +10105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>33</v>
       </c>
@@ -10128,7 +10128,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>34</v>
       </c>
@@ -10151,7 +10151,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>35</v>
       </c>
@@ -10174,7 +10174,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>36</v>
       </c>
@@ -10197,7 +10197,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>37</v>
       </c>
@@ -10220,7 +10220,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>38</v>
       </c>
@@ -10243,7 +10243,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>39</v>
       </c>
@@ -10266,7 +10266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>40</v>
       </c>
@@ -10289,7 +10289,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>41</v>
       </c>
@@ -10312,7 +10312,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>42</v>
       </c>
@@ -10335,7 +10335,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>43</v>
       </c>
@@ -10358,7 +10358,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>44</v>
       </c>
@@ -10381,7 +10381,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>45</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>46</v>
       </c>
@@ -10427,7 +10427,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>47</v>
       </c>
@@ -10450,7 +10450,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>48</v>
       </c>
@@ -10473,7 +10473,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>49</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>50</v>
       </c>
@@ -10519,7 +10519,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>51</v>
       </c>
@@ -10542,7 +10542,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>58</v>
       </c>
@@ -10565,7 +10565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>59</v>
       </c>
@@ -10588,7 +10588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>66</v>
       </c>
@@ -10611,7 +10611,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>67</v>
       </c>
@@ -10634,7 +10634,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>68</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>69</v>
       </c>
@@ -10680,7 +10680,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>70</v>
       </c>
@@ -10703,7 +10703,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>71</v>
       </c>
@@ -10726,7 +10726,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>72</v>
       </c>
@@ -10749,7 +10749,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>73</v>
       </c>
@@ -10772,7 +10772,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>74</v>
       </c>
@@ -10795,7 +10795,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>75</v>
       </c>
@@ -10818,7 +10818,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>76</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>77</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>78</v>
       </c>
@@ -10887,7 +10887,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>79</v>
       </c>
@@ -10919,7 +10919,7 @@
         <v>44686</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>83</v>
       </c>
@@ -10942,7 +10942,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>85</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>86</v>
       </c>
@@ -10988,7 +10988,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>87</v>
       </c>
@@ -11011,7 +11011,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>88</v>
       </c>
@@ -11034,7 +11034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>89</v>
       </c>
@@ -11057,7 +11057,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>90</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>91</v>
       </c>
@@ -11103,7 +11103,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>92</v>
       </c>
@@ -11126,7 +11126,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>93</v>
       </c>
@@ -11149,7 +11149,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>94</v>
       </c>
@@ -11172,7 +11172,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>95</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>96</v>
       </c>
@@ -11218,7 +11218,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>97</v>
       </c>
@@ -11241,7 +11241,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>98</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>99</v>
       </c>
@@ -11287,7 +11287,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>100</v>
       </c>
@@ -11310,7 +11310,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>101</v>
       </c>
@@ -11333,7 +11333,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>102</v>
       </c>
@@ -11356,7 +11356,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>103</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>104</v>
       </c>
@@ -11402,7 +11402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>105</v>
       </c>
@@ -11425,7 +11425,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>106</v>
       </c>
@@ -11448,7 +11448,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>107</v>
       </c>
@@ -11471,7 +11471,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>108</v>
       </c>
@@ -11494,7 +11494,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>109</v>
       </c>
@@ -11517,7 +11517,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>110</v>
       </c>
@@ -11540,7 +11540,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>111</v>
       </c>
@@ -11563,7 +11563,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>112</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>113</v>
       </c>
@@ -11609,7 +11609,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>114</v>
       </c>
@@ -11632,7 +11632,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>115</v>
       </c>
@@ -11655,7 +11655,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>116</v>
       </c>
@@ -11678,7 +11678,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>117</v>
       </c>
@@ -11701,7 +11701,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>118</v>
       </c>
@@ -11724,7 +11724,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>119</v>
       </c>
@@ -11747,7 +11747,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>120</v>
       </c>
@@ -11770,7 +11770,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>121</v>
       </c>
@@ -11793,7 +11793,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>122</v>
       </c>
@@ -11816,7 +11816,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>123</v>
       </c>
@@ -11839,7 +11839,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>132</v>
       </c>
@@ -11862,7 +11862,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>133</v>
       </c>
@@ -11885,7 +11885,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>134</v>
       </c>
@@ -11908,7 +11908,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>135</v>
       </c>
@@ -11931,7 +11931,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>136</v>
       </c>
@@ -11954,7 +11954,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>137</v>
       </c>
@@ -11977,7 +11977,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>138</v>
       </c>
@@ -12000,7 +12000,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>139</v>
       </c>
@@ -12023,7 +12023,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>172</v>
       </c>
@@ -12046,7 +12046,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>173</v>
       </c>
@@ -12069,7 +12069,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>174</v>
       </c>
@@ -12092,7 +12092,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>175</v>
       </c>
@@ -12115,7 +12115,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>176</v>
       </c>
@@ -12138,7 +12138,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>177</v>
       </c>
@@ -12161,7 +12161,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>178</v>
       </c>
@@ -12184,7 +12184,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>179</v>
       </c>
@@ -12207,7 +12207,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>180</v>
       </c>
@@ -12230,7 +12230,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>181</v>
       </c>
@@ -12253,7 +12253,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>182</v>
       </c>
@@ -12276,7 +12276,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>195</v>
       </c>
@@ -12299,7 +12299,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>196</v>
       </c>
@@ -12322,7 +12322,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>198</v>
       </c>
@@ -12345,7 +12345,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>199</v>
       </c>
@@ -12368,7 +12368,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>200</v>
       </c>
@@ -12391,7 +12391,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>201</v>
       </c>
@@ -12414,7 +12414,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>214</v>
       </c>
@@ -12437,7 +12437,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>215</v>
       </c>
@@ -12460,7 +12460,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>216</v>
       </c>
@@ -12483,7 +12483,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>217</v>
       </c>
@@ -12506,7 +12506,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>218</v>
       </c>
@@ -12529,7 +12529,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>219</v>
       </c>
@@ -12552,7 +12552,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>220</v>
       </c>
@@ -12575,7 +12575,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>221</v>
       </c>
@@ -12598,7 +12598,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>222</v>
       </c>
@@ -12621,7 +12621,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>223</v>
       </c>
@@ -12644,7 +12644,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>224</v>
       </c>
@@ -12667,7 +12667,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>225</v>
       </c>
@@ -12690,7 +12690,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>226</v>
       </c>
@@ -12713,7 +12713,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>227</v>
       </c>
@@ -12736,7 +12736,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>228</v>
       </c>
@@ -12759,7 +12759,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>229</v>
       </c>
@@ -12782,7 +12782,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>230</v>
       </c>
@@ -12805,7 +12805,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>231</v>
       </c>
@@ -12828,7 +12828,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>232</v>
       </c>
@@ -12851,7 +12851,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>233</v>
       </c>
@@ -12874,7 +12874,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>234</v>
       </c>
@@ -12897,7 +12897,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>236</v>
       </c>
@@ -12920,7 +12920,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>237</v>
       </c>
@@ -12943,7 +12943,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>238</v>
       </c>
@@ -12966,7 +12966,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>239</v>
       </c>
@@ -12989,7 +12989,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>240</v>
       </c>
@@ -13012,7 +13012,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>256</v>
       </c>
@@ -13035,7 +13035,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>257</v>
       </c>
@@ -13058,7 +13058,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>258</v>
       </c>
@@ -13081,7 +13081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>259</v>
       </c>
@@ -13104,7 +13104,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>260</v>
       </c>
@@ -13127,7 +13127,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>261</v>
       </c>
@@ -13150,7 +13150,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>262</v>
       </c>
@@ -13173,7 +13173,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>263</v>
       </c>
@@ -13196,7 +13196,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>264</v>
       </c>
@@ -13219,7 +13219,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>265</v>
       </c>
@@ -13242,7 +13242,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>282</v>
       </c>
@@ -13265,7 +13265,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>283</v>
       </c>
@@ -13288,7 +13288,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>284</v>
       </c>
@@ -13311,7 +13311,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>287</v>
       </c>
@@ -13334,7 +13334,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>289</v>
       </c>
@@ -13357,7 +13357,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>291</v>
       </c>
@@ -13380,7 +13380,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>293</v>
       </c>
@@ -13403,7 +13403,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>294</v>
       </c>
@@ -13426,7 +13426,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>295</v>
       </c>
@@ -13449,7 +13449,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>296</v>
       </c>
@@ -13472,7 +13472,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>297</v>
       </c>
@@ -13495,7 +13495,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>298</v>
       </c>
@@ -13518,7 +13518,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>299</v>
       </c>
@@ -13541,7 +13541,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>300</v>
       </c>
@@ -13564,7 +13564,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>301</v>
       </c>
@@ -13587,7 +13587,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>302</v>
       </c>
@@ -13610,7 +13610,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>303</v>
       </c>
@@ -13633,7 +13633,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>304</v>
       </c>
@@ -13656,7 +13656,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>305</v>
       </c>
@@ -13679,7 +13679,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>306</v>
       </c>
@@ -13702,7 +13702,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>307</v>
       </c>
@@ -13725,7 +13725,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>308</v>
       </c>
@@ -13748,7 +13748,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>309</v>
       </c>
@@ -13771,7 +13771,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>310</v>
       </c>
@@ -13794,7 +13794,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>311</v>
       </c>
@@ -13817,7 +13817,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>312</v>
       </c>
@@ -13840,7 +13840,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>313</v>
       </c>
@@ -13863,7 +13863,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>314</v>
       </c>
@@ -13886,7 +13886,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>315</v>
       </c>
@@ -13909,7 +13909,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>316</v>
       </c>
@@ -13932,7 +13932,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>317</v>
       </c>
@@ -13955,7 +13955,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>318</v>
       </c>
@@ -13978,7 +13978,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>319</v>
       </c>
@@ -14001,7 +14001,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>320</v>
       </c>
@@ -14024,7 +14024,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>321</v>
       </c>
@@ -14047,7 +14047,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>322</v>
       </c>
@@ -14070,7 +14070,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>323</v>
       </c>
@@ -14093,7 +14093,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>339</v>
       </c>
@@ -14116,7 +14116,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>340</v>
       </c>
@@ -14139,7 +14139,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>341</v>
       </c>
@@ -14162,7 +14162,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>342</v>
       </c>
@@ -14185,7 +14185,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>343</v>
       </c>
@@ -14208,7 +14208,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>344</v>
       </c>
@@ -14231,7 +14231,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>362</v>
       </c>
@@ -14254,7 +14254,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>363</v>
       </c>
@@ -14277,7 +14277,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>364</v>
       </c>
@@ -14300,7 +14300,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>365</v>
       </c>
@@ -14323,7 +14323,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>366</v>
       </c>
@@ -14346,7 +14346,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>367</v>
       </c>
@@ -14369,7 +14369,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>368</v>
       </c>
@@ -14392,7 +14392,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>369</v>
       </c>
@@ -14415,7 +14415,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>378</v>
       </c>
@@ -14438,7 +14438,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>379</v>
       </c>
@@ -14461,7 +14461,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>381</v>
       </c>
@@ -14484,7 +14484,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>383</v>
       </c>
@@ -14507,7 +14507,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>384</v>
       </c>
@@ -14530,7 +14530,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
         <v>385</v>
       </c>
@@ -14553,7 +14553,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
         <v>386</v>
       </c>
@@ -14576,7 +14576,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
         <v>389</v>
       </c>
@@ -14599,7 +14599,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="1">
         <v>390</v>
       </c>
@@ -14622,7 +14622,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="1">
         <v>392</v>
       </c>
@@ -14645,7 +14645,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" s="1">
         <v>393</v>
       </c>
@@ -14668,7 +14668,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" s="1">
         <v>394</v>
       </c>
@@ -14691,7 +14691,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" s="1">
         <v>404</v>
       </c>
@@ -14714,7 +14714,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" s="1">
         <v>405</v>
       </c>
@@ -14737,7 +14737,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" s="1">
         <v>406</v>
       </c>
@@ -14760,7 +14760,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" s="1">
         <v>413</v>
       </c>
@@ -14783,7 +14783,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" s="1">
         <v>414</v>
       </c>
@@ -14806,7 +14806,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" s="1">
         <v>415</v>
       </c>
@@ -14829,7 +14829,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
         <v>416</v>
       </c>
@@ -14852,7 +14852,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
         <v>417</v>
       </c>
@@ -14875,7 +14875,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
         <v>418</v>
       </c>
@@ -14898,7 +14898,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" s="1">
         <v>419</v>
       </c>
@@ -14921,7 +14921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" s="1">
         <v>420</v>
       </c>
@@ -14944,7 +14944,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" s="1">
         <v>421</v>
       </c>
@@ -14967,7 +14967,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" s="1">
         <v>422</v>
       </c>
@@ -14990,7 +14990,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" s="1">
         <v>423</v>
       </c>
@@ -15013,7 +15013,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
         <v>424</v>
       </c>
@@ -15036,7 +15036,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
         <v>425</v>
       </c>
@@ -15059,7 +15059,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
         <v>426</v>
       </c>
@@ -15082,7 +15082,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
         <v>427</v>
       </c>
@@ -15105,7 +15105,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" s="1">
         <v>428</v>
       </c>
@@ -15128,7 +15128,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
         <v>429</v>
       </c>
@@ -15151,7 +15151,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
         <v>430</v>
       </c>
@@ -15174,7 +15174,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
         <v>431</v>
       </c>
@@ -15197,7 +15197,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>432</v>
       </c>
@@ -15220,7 +15220,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" s="1">
         <v>433</v>
       </c>
@@ -15243,7 +15243,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
         <v>440</v>
       </c>
@@ -15266,7 +15266,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A245" s="1">
         <v>441</v>
       </c>
@@ -15289,7 +15289,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A246" s="1">
         <v>442</v>
       </c>
@@ -15312,7 +15312,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247" s="1">
         <v>443</v>
       </c>
@@ -15335,7 +15335,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248" s="1">
         <v>444</v>
       </c>
@@ -15358,7 +15358,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" s="1">
         <v>445</v>
       </c>
@@ -15381,7 +15381,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250" s="1">
         <v>459</v>
       </c>
@@ -15404,7 +15404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" s="1">
         <v>460</v>
       </c>
@@ -15427,7 +15427,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A252" s="1">
         <v>461</v>
       </c>
@@ -15450,7 +15450,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A253" s="1">
         <v>468</v>
       </c>
@@ -15473,7 +15473,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A254" s="1">
         <v>469</v>
       </c>
@@ -15496,7 +15496,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255" s="1">
         <v>470</v>
       </c>
@@ -15519,7 +15519,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A256" s="1">
         <v>471</v>
       </c>
@@ -15542,7 +15542,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A257" s="1">
         <v>477</v>
       </c>
@@ -15565,7 +15565,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A258" s="1">
         <v>478</v>
       </c>
@@ -15588,7 +15588,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A259" s="1">
         <v>479</v>
       </c>
@@ -15611,7 +15611,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A260" s="1">
         <v>480</v>
       </c>
@@ -15634,7 +15634,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261" s="1">
         <v>481</v>
       </c>
@@ -15657,7 +15657,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" s="1">
         <v>482</v>
       </c>
@@ -15680,7 +15680,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263" s="1">
         <v>483</v>
       </c>
@@ -15703,7 +15703,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" s="1">
         <v>484</v>
       </c>
@@ -15726,7 +15726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265" s="1">
         <v>485</v>
       </c>
@@ -15749,7 +15749,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266" s="1">
         <v>489</v>
       </c>
@@ -15772,7 +15772,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A267" s="1">
         <v>490</v>
       </c>
@@ -15795,7 +15795,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A268" s="1">
         <v>491</v>
       </c>
@@ -15818,7 +15818,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" s="1">
         <v>492</v>
       </c>
@@ -15841,7 +15841,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" s="1">
         <v>493</v>
       </c>
@@ -15864,7 +15864,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A271" s="1">
         <v>494</v>
       </c>
@@ -15887,7 +15887,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272" s="1">
         <v>495</v>
       </c>
@@ -15910,7 +15910,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" s="1">
         <v>496</v>
       </c>
@@ -15933,7 +15933,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274" s="1">
         <v>498</v>
       </c>
@@ -15956,7 +15956,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" s="1">
         <v>499</v>
       </c>
@@ -15979,7 +15979,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A276" s="1">
         <v>500</v>
       </c>
@@ -16002,7 +16002,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277" s="1">
         <v>501</v>
       </c>
@@ -16025,7 +16025,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A278" s="1">
         <v>502</v>
       </c>
@@ -16048,7 +16048,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A279" s="1">
         <v>503</v>
       </c>
@@ -16071,7 +16071,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A280" s="1">
         <v>504</v>
       </c>
@@ -16094,7 +16094,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A281" s="1">
         <v>520</v>
       </c>
@@ -16117,7 +16117,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A282" s="1">
         <v>521</v>
       </c>
@@ -16140,7 +16140,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A283" s="1">
         <v>524</v>
       </c>
@@ -16163,7 +16163,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A284" s="1">
         <v>526</v>
       </c>
@@ -16186,7 +16186,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A285" s="1">
         <v>527</v>
       </c>
@@ -16209,7 +16209,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A286" s="1">
         <v>531</v>
       </c>
@@ -16232,7 +16232,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A287" s="1">
         <v>533</v>
       </c>
@@ -16255,7 +16255,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A288" s="1">
         <v>534</v>
       </c>
@@ -16278,7 +16278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A289" s="1">
         <v>535</v>
       </c>
@@ -16301,7 +16301,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A290" s="1">
         <v>539</v>
       </c>
@@ -16324,7 +16324,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A291" s="1">
         <v>540</v>
       </c>
@@ -16347,7 +16347,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A292" s="1">
         <v>542</v>
       </c>
@@ -16370,7 +16370,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A293" s="1">
         <v>545</v>
       </c>
@@ -16393,7 +16393,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A294" s="1">
         <v>546</v>
       </c>
@@ -16416,7 +16416,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A295" s="1">
         <v>548</v>
       </c>
@@ -16439,7 +16439,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A296" s="1">
         <v>549</v>
       </c>
@@ -16462,7 +16462,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A297" s="1">
         <v>552</v>
       </c>
@@ -16485,7 +16485,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A298" s="1">
         <v>554</v>
       </c>
@@ -16508,7 +16508,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A299" s="1">
         <v>555</v>
       </c>
@@ -16531,7 +16531,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A300" s="1">
         <v>556</v>
       </c>
@@ -16554,7 +16554,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A301" s="1">
         <v>560</v>
       </c>
@@ -16577,7 +16577,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A302" s="1">
         <v>561</v>
       </c>
@@ -16600,7 +16600,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A303" s="1">
         <v>562</v>
       </c>
@@ -16623,7 +16623,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A304" s="1">
         <v>563</v>
       </c>
@@ -16646,7 +16646,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A305" s="1">
         <v>564</v>
       </c>
@@ -16669,7 +16669,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A306" s="1">
         <v>565</v>
       </c>
@@ -16692,7 +16692,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A307" s="1">
         <v>566</v>
       </c>
@@ -16715,7 +16715,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A308" s="1">
         <v>567</v>
       </c>
@@ -16738,7 +16738,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A309" s="1">
         <v>568</v>
       </c>
@@ -16761,7 +16761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A310" s="1">
         <v>569</v>
       </c>
@@ -16784,7 +16784,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A311" s="1">
         <v>570</v>
       </c>
@@ -16807,7 +16807,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A312" s="1">
         <v>571</v>
       </c>
@@ -16830,7 +16830,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A313" s="1">
         <v>572</v>
       </c>
@@ -16853,7 +16853,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A314" s="1">
         <v>573</v>
       </c>
@@ -16876,7 +16876,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A315" s="1">
         <v>575</v>
       </c>
@@ -16899,7 +16899,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A316" s="1">
         <v>576</v>
       </c>
@@ -16922,7 +16922,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A317" s="1">
         <v>577</v>
       </c>
@@ -16945,7 +16945,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A318" s="1">
         <v>578</v>
       </c>
@@ -16968,7 +16968,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A319" s="1">
         <v>579</v>
       </c>
@@ -16991,7 +16991,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A320" s="1">
         <v>580</v>
       </c>
@@ -17014,7 +17014,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A321" s="1">
         <v>581</v>
       </c>
@@ -17037,7 +17037,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A322" s="1">
         <v>582</v>
       </c>
@@ -17060,7 +17060,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A323" s="1">
         <v>584</v>
       </c>
@@ -17083,7 +17083,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A324" s="1">
         <v>585</v>
       </c>
@@ -17106,7 +17106,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A325" s="1">
         <v>586</v>
       </c>
@@ -17129,7 +17129,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A326" s="1">
         <v>587</v>
       </c>
@@ -17152,7 +17152,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A327" s="1">
         <v>588</v>
       </c>
@@ -17175,7 +17175,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A328" s="1">
         <v>591</v>
       </c>
@@ -17198,7 +17198,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A329" s="1">
         <v>592</v>
       </c>
@@ -17221,7 +17221,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A330" s="1">
         <v>598</v>
       </c>
@@ -17244,7 +17244,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A331" s="1">
         <v>599</v>
       </c>
@@ -17267,7 +17267,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A332" s="1">
         <v>600</v>
       </c>
@@ -17290,7 +17290,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A333" s="1">
         <v>601</v>
       </c>
@@ -17313,7 +17313,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="334" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A334" s="1">
         <v>602</v>
       </c>
@@ -17336,7 +17336,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A335" s="1">
         <v>603</v>
       </c>
@@ -17359,7 +17359,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A336" s="1">
         <v>604</v>
       </c>
@@ -17382,7 +17382,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A337" s="1">
         <v>605</v>
       </c>
@@ -17405,7 +17405,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A338" s="1">
         <v>606</v>
       </c>
@@ -17428,7 +17428,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A339" s="1">
         <v>607</v>
       </c>
@@ -17451,7 +17451,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A340" s="1">
         <v>608</v>
       </c>
@@ -17474,7 +17474,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A341" s="1">
         <v>609</v>
       </c>
@@ -17497,7 +17497,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A342" s="1">
         <v>610</v>
       </c>
@@ -17520,7 +17520,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A343" s="1">
         <v>611</v>
       </c>
@@ -17543,7 +17543,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A344" s="1">
         <v>612</v>
       </c>
@@ -17566,7 +17566,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A345" s="1">
         <v>613</v>
       </c>
@@ -17589,7 +17589,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A346" s="1">
         <v>621</v>
       </c>
@@ -17612,7 +17612,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A347" s="1">
         <v>622</v>
       </c>
@@ -17635,7 +17635,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A348" s="1">
         <v>627</v>
       </c>
@@ -17658,7 +17658,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A349" s="1">
         <v>628</v>
       </c>
@@ -17681,7 +17681,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A350" s="1">
         <v>629</v>
       </c>
@@ -17704,7 +17704,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A351" s="1">
         <v>630</v>
       </c>
@@ -17727,7 +17727,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A352" s="1">
         <v>631</v>
       </c>
@@ -17750,7 +17750,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A353" s="1">
         <v>632</v>
       </c>
@@ -17773,7 +17773,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A354" s="1">
         <v>633</v>
       </c>
@@ -17796,7 +17796,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A355" s="1">
         <v>634</v>
       </c>
@@ -17819,7 +17819,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A356" s="1">
         <v>635</v>
       </c>
@@ -17842,7 +17842,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A357" s="1">
         <v>636</v>
       </c>
@@ -17865,7 +17865,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A358" s="1">
         <v>637</v>
       </c>
@@ -17888,7 +17888,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A359" s="1">
         <v>638</v>
       </c>
@@ -17911,7 +17911,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A360" s="1">
         <v>639</v>
       </c>
@@ -17934,7 +17934,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A361" s="1">
         <v>640</v>
       </c>
@@ -17957,7 +17957,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A362" s="1">
         <v>641</v>
       </c>
@@ -17980,7 +17980,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A363" s="1">
         <v>642</v>
       </c>
@@ -18003,7 +18003,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A364" s="1">
         <v>643</v>
       </c>
@@ -18026,7 +18026,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A365" s="1">
         <v>644</v>
       </c>
@@ -18049,7 +18049,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A366" s="1">
         <v>645</v>
       </c>
@@ -18072,7 +18072,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A367" s="1">
         <v>646</v>
       </c>
@@ -18095,7 +18095,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A368" s="1">
         <v>647</v>
       </c>
@@ -18118,7 +18118,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A369" s="1">
         <v>648</v>
       </c>
@@ -18141,7 +18141,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A370" s="1">
         <v>650</v>
       </c>
@@ -18164,7 +18164,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A371" s="1">
         <v>651</v>
       </c>
@@ -18187,7 +18187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A372" s="1">
         <v>652</v>
       </c>
@@ -18210,7 +18210,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A373" s="1">
         <v>653</v>
       </c>
@@ -18233,7 +18233,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A374" s="1">
         <v>654</v>
       </c>
@@ -18256,7 +18256,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A375" s="1">
         <v>655</v>
       </c>
@@ -18279,7 +18279,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A376" s="1">
         <v>656</v>
       </c>
@@ -18302,7 +18302,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A377" s="1">
         <v>657</v>
       </c>
@@ -18325,7 +18325,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A378" s="1">
         <v>658</v>
       </c>
@@ -18348,7 +18348,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="379" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A379" s="1">
         <v>659</v>
       </c>
@@ -18371,7 +18371,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="380" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A380" s="1">
         <v>660</v>
       </c>
@@ -18394,7 +18394,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="381" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A381" s="1">
         <v>661</v>
       </c>
@@ -18417,7 +18417,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="382" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A382" s="1">
         <v>662</v>
       </c>
@@ -18440,7 +18440,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="383" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A383" s="1">
         <v>663</v>
       </c>
@@ -18463,7 +18463,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="384" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A384" s="1">
         <v>672</v>
       </c>
@@ -18486,7 +18486,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="385" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A385" s="1">
         <v>673</v>
       </c>
@@ -18509,7 +18509,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="386" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A386" s="1">
         <v>674</v>
       </c>
@@ -18532,7 +18532,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="387" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A387" s="1">
         <v>675</v>
       </c>
@@ -18555,7 +18555,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="388" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A388" s="1">
         <v>676</v>
       </c>
@@ -18578,7 +18578,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="389" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A389" s="1">
         <v>677</v>
       </c>
@@ -18601,7 +18601,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="390" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A390" s="1">
         <v>678</v>
       </c>
@@ -18624,7 +18624,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="391" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A391" s="1">
         <v>681</v>
       </c>
@@ -18647,7 +18647,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A392" s="1">
         <v>682</v>
       </c>
@@ -18670,7 +18670,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A393" s="1">
         <v>683</v>
       </c>
@@ -23246,7 +23246,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="551" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="551" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A551" s="1">
         <v>80</v>
       </c>
@@ -23279,6 +23279,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L551" xr:uid="{B6CD1FA5-7C40-4123-BBCD-AB20E1A16CDA}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Cosco"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="G30" r:id="rId1" xr:uid="{61C19AB0-F3C3-4C1A-A7CA-06DA5BC8E1CF}"/>
   </hyperlinks>
@@ -23887,21 +23894,21 @@
       <c r="E9" s="20" t="s">
         <v>587</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="39" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="36.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="C10" s="40"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="37"/>
       <c r="E10" s="15" t="s">
         <v>588</v>
       </c>
-      <c r="F10" s="42"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:6" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="33"/>
@@ -23933,7 +23940,7 @@
       <c r="E12" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="41" t="s">
         <v>600</v>
       </c>
     </row>
@@ -23945,7 +23952,7 @@
       <c r="C13" s="33"/>
       <c r="D13" s="37"/>
       <c r="E13" s="37"/>
-      <c r="F13" s="39"/>
+      <c r="F13" s="42"/>
     </row>
     <row r="14" spans="1:6" ht="36.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
@@ -24088,27 +24095,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://www.mtrtml.com/" xr:uid="{AE13F086-D27A-4C56-828B-0E594EBC2B3B}"/>

</xml_diff>